<commit_message>
recalc for diaz et al
</commit_message>
<xml_diff>
--- a/Output/data_for_BD_3.31.2021.xlsx
+++ b/Output/data_for_BD_3.31.2021.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasbaetge/GITHUB/naames_export_ms/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AFC37C-E18D-E849-B421-45B51AC0EE71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36329002-27D0-C943-9CA4-0CDB6DE948EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18980" yWindow="1440" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{C714C0BF-6981-B946-8CFC-AB0C95C9EFCA}"/>
+    <workbookView xWindow="2600" yWindow="1340" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{C714C0BF-6981-B946-8CFC-AB0C95C9EFCA}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
-    <sheet name="data" sheetId="6" r:id="rId2"/>
+    <sheet name="data" sheetId="7" r:id="rId2"/>
     <sheet name="summary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7879" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8129" uniqueCount="142">
   <si>
     <t>value</t>
   </si>
@@ -1110,7 +1110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128C6583-DD21-EA42-8689-5AD1295B5947}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171ED5D6-CC67-F14F-BFF4-C5929F42ABF4}">
   <dimension ref="A1:AE849"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1300,11 +1300,11 @@
       <c r="AC2">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD2">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE2">
-        <v>5.0903853773848899</v>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
@@ -1395,11 +1395,11 @@
       <c r="AC3">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD3">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE3">
-        <v>5.0903853773848899</v>
+      <c r="AD3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -1490,11 +1490,11 @@
       <c r="AC4">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD4">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE4">
-        <v>5.0903853773848899</v>
+      <c r="AD4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
@@ -1585,11 +1585,11 @@
       <c r="AC5">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD5">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE5">
-        <v>5.0903853773848899</v>
+      <c r="AD5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
@@ -1680,11 +1680,11 @@
       <c r="AC6">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD6">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE6">
-        <v>5.0903853773848899</v>
+      <c r="AD6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
@@ -1775,11 +1775,11 @@
       <c r="AC7">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD7">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE7">
-        <v>5.0903853773848899</v>
+      <c r="AD7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
@@ -1870,11 +1870,11 @@
       <c r="AC8">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD8">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE8">
-        <v>5.0903853773848899</v>
+      <c r="AD8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
@@ -1965,11 +1965,11 @@
       <c r="AC9">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD9">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE9">
-        <v>5.0903853773848899</v>
+      <c r="AD9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
@@ -2060,11 +2060,11 @@
       <c r="AC10">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD10">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE10">
-        <v>5.0903853773848899</v>
+      <c r="AD10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
@@ -2155,11 +2155,11 @@
       <c r="AC11">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD11">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE11">
-        <v>5.0903853773848899</v>
+      <c r="AD11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
@@ -2250,11 +2250,11 @@
       <c r="AC12">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD12">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE12">
-        <v>5.0903853773848899</v>
+      <c r="AD12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
@@ -2345,11 +2345,11 @@
       <c r="AC13">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD13">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE13">
-        <v>5.0903853773848899</v>
+      <c r="AD13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
@@ -2440,11 +2440,11 @@
       <c r="AC14">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD14">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE14">
-        <v>5.0903853773848899</v>
+      <c r="AD14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
@@ -2535,11 +2535,11 @@
       <c r="AC15">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD15">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE15">
-        <v>5.0903853773848899</v>
+      <c r="AD15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
@@ -2630,11 +2630,11 @@
       <c r="AC16">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD16">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE16">
-        <v>5.0903853773848899</v>
+      <c r="AD16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
@@ -2725,11 +2725,11 @@
       <c r="AC17">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD17">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE17">
-        <v>5.0903853773848899</v>
+      <c r="AD17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
@@ -2820,11 +2820,11 @@
       <c r="AC18">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD18">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE18">
-        <v>5.0903853773848899</v>
+      <c r="AD18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
@@ -2915,11 +2915,11 @@
       <c r="AC19">
         <v>52.239162497616498</v>
       </c>
-      <c r="AD19">
-        <v>5.1883511657323602</v>
-      </c>
-      <c r="AE19">
-        <v>5.0903853773848899</v>
+      <c r="AD19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
@@ -3010,11 +3010,11 @@
       <c r="AC20">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD20">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE20">
-        <v>1.6290997451478799</v>
+      <c r="AD20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
@@ -3105,11 +3105,11 @@
       <c r="AC21">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD21">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE21">
-        <v>1.6290997451478799</v>
+      <c r="AD21" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
@@ -3200,11 +3200,11 @@
       <c r="AC22">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD22">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE22">
-        <v>1.6290997451478799</v>
+      <c r="AD22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
@@ -3295,11 +3295,11 @@
       <c r="AC23">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD23">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE23">
-        <v>1.6290997451478799</v>
+      <c r="AD23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
@@ -3390,11 +3390,11 @@
       <c r="AC24">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD24">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE24">
-        <v>1.6290997451478799</v>
+      <c r="AD24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
@@ -3485,11 +3485,11 @@
       <c r="AC25">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD25">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE25">
-        <v>1.6290997451478799</v>
+      <c r="AD25" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
@@ -3580,11 +3580,11 @@
       <c r="AC26">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD26">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE26">
-        <v>1.6290997451478799</v>
+      <c r="AD26" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
@@ -3675,11 +3675,11 @@
       <c r="AC27">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD27">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE27">
-        <v>1.6290997451478799</v>
+      <c r="AD27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
@@ -3770,11 +3770,11 @@
       <c r="AC28">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD28">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE28">
-        <v>1.6290997451478799</v>
+      <c r="AD28" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
@@ -3865,11 +3865,11 @@
       <c r="AC29">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD29">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE29">
-        <v>1.6290997451478799</v>
+      <c r="AD29" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
@@ -3960,11 +3960,11 @@
       <c r="AC30">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD30">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE30">
-        <v>1.6290997451478799</v>
+      <c r="AD30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
@@ -4055,11 +4055,11 @@
       <c r="AC31">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD31">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE31">
-        <v>1.6290997451478799</v>
+      <c r="AD31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
@@ -4150,11 +4150,11 @@
       <c r="AC32">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD32">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE32">
-        <v>1.6290997451478799</v>
+      <c r="AD32" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
@@ -4245,11 +4245,11 @@
       <c r="AC33">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD33">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE33">
-        <v>1.6290997451478799</v>
+      <c r="AD33" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
@@ -4340,11 +4340,11 @@
       <c r="AC34">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD34">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE34">
-        <v>1.6290997451478799</v>
+      <c r="AD34" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
@@ -4435,11 +4435,11 @@
       <c r="AC35">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD35">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE35">
-        <v>1.6290997451478799</v>
+      <c r="AD35" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
@@ -4530,11 +4530,11 @@
       <c r="AC36">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD36">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE36">
-        <v>1.6290997451478799</v>
+      <c r="AD36" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
@@ -4625,11 +4625,11 @@
       <c r="AC37">
         <v>51.828035894890803</v>
       </c>
-      <c r="AD37">
-        <v>1.75371868829865</v>
-      </c>
-      <c r="AE37">
-        <v>1.6290997451478799</v>
+      <c r="AD37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
@@ -4720,11 +4720,11 @@
       <c r="AC38">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD38">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE38">
-        <v>6.8712852399084197</v>
+      <c r="AD38" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
@@ -4815,11 +4815,11 @@
       <c r="AC39">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD39">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE39">
-        <v>6.8712852399084197</v>
+      <c r="AD39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
@@ -4910,11 +4910,11 @@
       <c r="AC40">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD40">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE40">
-        <v>6.8712852399084197</v>
+      <c r="AD40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
@@ -5005,11 +5005,11 @@
       <c r="AC41">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD41">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE41">
-        <v>6.8712852399084197</v>
+      <c r="AD41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
@@ -5100,11 +5100,11 @@
       <c r="AC42">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD42">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE42">
-        <v>6.8712852399084197</v>
+      <c r="AD42" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
@@ -5195,11 +5195,11 @@
       <c r="AC43">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD43">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE43">
-        <v>6.8712852399084197</v>
+      <c r="AD43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
@@ -5290,11 +5290,11 @@
       <c r="AC44">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD44">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE44">
-        <v>6.8712852399084197</v>
+      <c r="AD44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
@@ -5385,11 +5385,11 @@
       <c r="AC45">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD45">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE45">
-        <v>6.8712852399084197</v>
+      <c r="AD45" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
@@ -5480,11 +5480,11 @@
       <c r="AC46">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD46">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE46">
-        <v>6.8712852399084197</v>
+      <c r="AD46" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
@@ -5575,11 +5575,11 @@
       <c r="AC47">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD47">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE47">
-        <v>6.8712852399084197</v>
+      <c r="AD47" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
@@ -5670,11 +5670,11 @@
       <c r="AC48">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD48">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE48">
-        <v>6.8712852399084197</v>
+      <c r="AD48" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.2">
@@ -5765,11 +5765,11 @@
       <c r="AC49">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD49">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE49">
-        <v>6.8712852399084197</v>
+      <c r="AD49" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.2">
@@ -5860,11 +5860,11 @@
       <c r="AC50">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD50">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE50">
-        <v>6.8712852399084197</v>
+      <c r="AD50" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.2">
@@ -5955,11 +5955,11 @@
       <c r="AC51">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD51">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE51">
-        <v>6.8712852399084197</v>
+      <c r="AD51" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.2">
@@ -6050,11 +6050,11 @@
       <c r="AC52">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD52">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE52">
-        <v>6.8712852399084197</v>
+      <c r="AD52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.2">
@@ -6145,11 +6145,11 @@
       <c r="AC53">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD53">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE53">
-        <v>6.8712852399084197</v>
+      <c r="AD53" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.2">
@@ -6240,11 +6240,11 @@
       <c r="AC54">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD54">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE54">
-        <v>6.8712852399084197</v>
+      <c r="AD54" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.2">
@@ -6335,11 +6335,11 @@
       <c r="AC55">
         <v>51.536150898341901</v>
       </c>
-      <c r="AD55">
-        <v>7.0471521971220596</v>
-      </c>
-      <c r="AE55">
-        <v>6.8712852399084197</v>
+      <c r="AD55" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.2">
@@ -6430,11 +6430,11 @@
       <c r="AC56">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD56">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE56">
-        <v>3.6967897166007901</v>
+      <c r="AD56" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.2">
@@ -6525,11 +6525,11 @@
       <c r="AC57">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD57">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE57">
-        <v>3.6967897166007901</v>
+      <c r="AD57" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.2">
@@ -6620,11 +6620,11 @@
       <c r="AC58">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD58">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE58">
-        <v>3.6967897166007901</v>
+      <c r="AD58" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.2">
@@ -6715,11 +6715,11 @@
       <c r="AC59">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD59">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE59">
-        <v>3.6967897166007901</v>
+      <c r="AD59" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.2">
@@ -6810,11 +6810,11 @@
       <c r="AC60">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD60">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE60">
-        <v>3.6967897166007901</v>
+      <c r="AD60" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.2">
@@ -6905,11 +6905,11 @@
       <c r="AC61">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD61">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE61">
-        <v>3.6967897166007901</v>
+      <c r="AD61" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.2">
@@ -7000,11 +7000,11 @@
       <c r="AC62">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD62">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE62">
-        <v>3.6967897166007901</v>
+      <c r="AD62" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE62" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.2">
@@ -7095,11 +7095,11 @@
       <c r="AC63">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD63">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE63">
-        <v>3.6967897166007901</v>
+      <c r="AD63" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.2">
@@ -7190,11 +7190,11 @@
       <c r="AC64">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD64">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE64">
-        <v>3.6967897166007901</v>
+      <c r="AD64" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE64" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.2">
@@ -7285,11 +7285,11 @@
       <c r="AC65">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD65">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE65">
-        <v>3.6967897166007901</v>
+      <c r="AD65" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.2">
@@ -7380,11 +7380,11 @@
       <c r="AC66">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD66">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE66">
-        <v>3.6967897166007901</v>
+      <c r="AD66" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.2">
@@ -7475,11 +7475,11 @@
       <c r="AC67">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD67">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE67">
-        <v>3.6967897166007901</v>
+      <c r="AD67" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.2">
@@ -7570,11 +7570,11 @@
       <c r="AC68">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD68">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE68">
-        <v>3.6967897166007901</v>
+      <c r="AD68" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.2">
@@ -7665,11 +7665,11 @@
       <c r="AC69">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD69">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE69">
-        <v>3.6967897166007901</v>
+      <c r="AD69" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.2">
@@ -7760,11 +7760,11 @@
       <c r="AC70">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD70">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE70">
-        <v>3.6967897166007901</v>
+      <c r="AD70" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE70" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.2">
@@ -7855,11 +7855,11 @@
       <c r="AC71">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD71">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE71">
-        <v>3.6967897166007901</v>
+      <c r="AD71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.2">
@@ -7950,11 +7950,11 @@
       <c r="AC72">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD72">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE72">
-        <v>3.6967897166007901</v>
+      <c r="AD72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.2">
@@ -8045,11 +8045,11 @@
       <c r="AC73">
         <v>53.941204450288403</v>
       </c>
-      <c r="AD73">
-        <v>3.8342652033340801</v>
-      </c>
-      <c r="AE73">
-        <v>3.6967897166007901</v>
+      <c r="AD73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE73" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.2">
@@ -8140,11 +8140,11 @@
       <c r="AC74">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD74">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE74">
-        <v>34.975700391659601</v>
+      <c r="AD74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.2">
@@ -8235,11 +8235,11 @@
       <c r="AC75">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD75">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE75">
-        <v>34.975700391659601</v>
+      <c r="AD75" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE75" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.2">
@@ -8330,11 +8330,11 @@
       <c r="AC76">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD76">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE76">
-        <v>34.975700391659601</v>
+      <c r="AD76" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE76" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.2">
@@ -8425,11 +8425,11 @@
       <c r="AC77">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD77">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE77">
-        <v>34.975700391659601</v>
+      <c r="AD77" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE77" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.2">
@@ -8520,11 +8520,11 @@
       <c r="AC78">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD78">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE78">
-        <v>34.975700391659601</v>
+      <c r="AD78" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE78" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.2">
@@ -8615,11 +8615,11 @@
       <c r="AC79">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD79">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE79">
-        <v>34.975700391659601</v>
+      <c r="AD79" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE79" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.2">
@@ -8710,11 +8710,11 @@
       <c r="AC80">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD80">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE80">
-        <v>34.975700391659601</v>
+      <c r="AD80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE80" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.2">
@@ -8805,11 +8805,11 @@
       <c r="AC81">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD81">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE81">
-        <v>34.975700391659601</v>
+      <c r="AD81" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE81" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.2">
@@ -8900,11 +8900,11 @@
       <c r="AC82">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD82">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE82">
-        <v>34.975700391659601</v>
+      <c r="AD82" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE82" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.2">
@@ -8995,11 +8995,11 @@
       <c r="AC83">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD83">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE83">
-        <v>34.975700391659601</v>
+      <c r="AD83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE83" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.2">
@@ -9090,11 +9090,11 @@
       <c r="AC84">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD84">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE84">
-        <v>34.975700391659601</v>
+      <c r="AD84" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE84" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.2">
@@ -9185,11 +9185,11 @@
       <c r="AC85">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD85">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE85">
-        <v>34.975700391659601</v>
+      <c r="AD85" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE85" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.2">
@@ -9280,11 +9280,11 @@
       <c r="AC86">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD86">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE86">
-        <v>34.975700391659601</v>
+      <c r="AD86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE86" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.2">
@@ -9375,11 +9375,11 @@
       <c r="AC87">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD87">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE87">
-        <v>34.975700391659601</v>
+      <c r="AD87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE87" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.2">
@@ -9470,11 +9470,11 @@
       <c r="AC88">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD88">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE88">
-        <v>34.975700391659601</v>
+      <c r="AD88" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE88" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.2">
@@ -9565,11 +9565,11 @@
       <c r="AC89">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD89">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE89">
-        <v>34.975700391659601</v>
+      <c r="AD89" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE89" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.2">
@@ -9660,11 +9660,11 @@
       <c r="AC90">
         <v>52.365951030815197</v>
       </c>
-      <c r="AD90">
-        <v>35.608743290881897</v>
-      </c>
-      <c r="AE90">
-        <v>34.975700391659601</v>
+      <c r="AD90" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE90" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.2">
@@ -9755,11 +9755,11 @@
       <c r="AC91">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD91">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE91">
-        <v>5.2592701496162899</v>
+      <c r="AD91" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE91" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.2">
@@ -9850,11 +9850,11 @@
       <c r="AC92">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD92">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE92">
-        <v>5.2592701496162899</v>
+      <c r="AD92" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE92" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.2">
@@ -9945,11 +9945,11 @@
       <c r="AC93">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD93">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE93">
-        <v>5.2592701496162899</v>
+      <c r="AD93" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE93" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.2">
@@ -10040,11 +10040,11 @@
       <c r="AC94">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD94">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE94">
-        <v>5.2592701496162899</v>
+      <c r="AD94" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE94" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.2">
@@ -10135,11 +10135,11 @@
       <c r="AC95">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD95">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE95">
-        <v>5.2592701496162899</v>
+      <c r="AD95" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE95" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.2">
@@ -10230,11 +10230,11 @@
       <c r="AC96">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD96">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE96">
-        <v>5.2592701496162899</v>
+      <c r="AD96" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE96" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.2">
@@ -10325,11 +10325,11 @@
       <c r="AC97">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD97">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE97">
-        <v>5.2592701496162899</v>
+      <c r="AD97" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE97" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.2">
@@ -10420,11 +10420,11 @@
       <c r="AC98">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD98">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE98">
-        <v>5.2592701496162899</v>
+      <c r="AD98" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE98" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.2">
@@ -10515,11 +10515,11 @@
       <c r="AC99">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD99">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE99">
-        <v>5.2592701496162899</v>
+      <c r="AD99" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE99" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.2">
@@ -10610,11 +10610,11 @@
       <c r="AC100">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD100">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE100">
-        <v>5.2592701496162899</v>
+      <c r="AD100" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE100" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.2">
@@ -10705,11 +10705,11 @@
       <c r="AC101">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD101">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE101">
-        <v>5.2592701496162899</v>
+      <c r="AD101" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE101" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.2">
@@ -10800,11 +10800,11 @@
       <c r="AC102">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD102">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE102">
-        <v>5.2592701496162899</v>
+      <c r="AD102" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE102" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.2">
@@ -10895,11 +10895,11 @@
       <c r="AC103">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD103">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE103">
-        <v>5.2592701496162899</v>
+      <c r="AD103" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE103" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.2">
@@ -10990,11 +10990,11 @@
       <c r="AC104">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD104">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE104">
-        <v>5.2592701496162899</v>
+      <c r="AD104" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE104" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.2">
@@ -11085,11 +11085,11 @@
       <c r="AC105">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD105">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE105">
-        <v>5.2592701496162899</v>
+      <c r="AD105" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE105" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.2">
@@ -11180,11 +11180,11 @@
       <c r="AC106">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD106">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE106">
-        <v>5.2592701496162899</v>
+      <c r="AD106" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE106" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.2">
@@ -11275,11 +11275,11 @@
       <c r="AC107">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD107">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE107">
-        <v>5.2592701496162899</v>
+      <c r="AD107" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE107" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.2">
@@ -11370,11 +11370,11 @@
       <c r="AC108">
         <v>53.494291253004803</v>
       </c>
-      <c r="AD108">
-        <v>5.36919117902195</v>
-      </c>
-      <c r="AE108">
-        <v>5.2592701496162899</v>
+      <c r="AD108" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE108" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.2">
@@ -13080,11 +13080,11 @@
       <c r="AC126">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD126">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE126">
-        <v>18.684312463162001</v>
+      <c r="AD126" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE126" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="127" spans="1:31" x14ac:dyDescent="0.2">
@@ -13175,11 +13175,11 @@
       <c r="AC127">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD127">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE127">
-        <v>18.684312463162001</v>
+      <c r="AD127" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE127" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="128" spans="1:31" x14ac:dyDescent="0.2">
@@ -13270,11 +13270,11 @@
       <c r="AC128">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD128">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE128">
-        <v>18.684312463162001</v>
+      <c r="AD128" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE128" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="129" spans="1:31" x14ac:dyDescent="0.2">
@@ -13365,11 +13365,11 @@
       <c r="AC129">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD129">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE129">
-        <v>18.684312463162001</v>
+      <c r="AD129" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE129" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="130" spans="1:31" x14ac:dyDescent="0.2">
@@ -13460,11 +13460,11 @@
       <c r="AC130">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD130">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE130">
-        <v>18.684312463162001</v>
+      <c r="AD130" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE130" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="131" spans="1:31" x14ac:dyDescent="0.2">
@@ -13555,11 +13555,11 @@
       <c r="AC131">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD131">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE131">
-        <v>18.684312463162001</v>
+      <c r="AD131" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE131" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="132" spans="1:31" x14ac:dyDescent="0.2">
@@ -13650,11 +13650,11 @@
       <c r="AC132">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD132">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE132">
-        <v>18.684312463162001</v>
+      <c r="AD132" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE132" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="133" spans="1:31" x14ac:dyDescent="0.2">
@@ -13745,11 +13745,11 @@
       <c r="AC133">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD133">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE133">
-        <v>18.684312463162001</v>
+      <c r="AD133" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE133" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="134" spans="1:31" x14ac:dyDescent="0.2">
@@ -13840,11 +13840,11 @@
       <c r="AC134">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD134">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE134">
-        <v>18.684312463162001</v>
+      <c r="AD134" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE134" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="135" spans="1:31" x14ac:dyDescent="0.2">
@@ -13935,11 +13935,11 @@
       <c r="AC135">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD135">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE135">
-        <v>18.684312463162001</v>
+      <c r="AD135" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE135" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="136" spans="1:31" x14ac:dyDescent="0.2">
@@ -14030,11 +14030,11 @@
       <c r="AC136">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD136">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE136">
-        <v>18.684312463162001</v>
+      <c r="AD136" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE136" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="137" spans="1:31" x14ac:dyDescent="0.2">
@@ -14125,11 +14125,11 @@
       <c r="AC137">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD137">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE137">
-        <v>18.684312463162001</v>
+      <c r="AD137" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE137" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="138" spans="1:31" x14ac:dyDescent="0.2">
@@ -14220,11 +14220,11 @@
       <c r="AC138">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD138">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE138">
-        <v>18.684312463162001</v>
+      <c r="AD138" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE138" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="139" spans="1:31" x14ac:dyDescent="0.2">
@@ -14315,11 +14315,11 @@
       <c r="AC139">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD139">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE139">
-        <v>18.684312463162001</v>
+      <c r="AD139" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE139" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="140" spans="1:31" x14ac:dyDescent="0.2">
@@ -14410,11 +14410,11 @@
       <c r="AC140">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD140">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE140">
-        <v>18.684312463162001</v>
+      <c r="AD140" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE140" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="141" spans="1:31" x14ac:dyDescent="0.2">
@@ -14505,11 +14505,11 @@
       <c r="AC141">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD141">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE141">
-        <v>18.684312463162001</v>
+      <c r="AD141" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE141" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="142" spans="1:31" x14ac:dyDescent="0.2">
@@ -14600,11 +14600,11 @@
       <c r="AC142">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD142">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE142">
-        <v>18.684312463162001</v>
+      <c r="AD142" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE142" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:31" x14ac:dyDescent="0.2">
@@ -14695,11 +14695,11 @@
       <c r="AC143">
         <v>52.883491148264397</v>
       </c>
-      <c r="AD143">
-        <v>19.406118422082301</v>
-      </c>
-      <c r="AE143">
-        <v>18.684312463162001</v>
+      <c r="AD143" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE143" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="144" spans="1:31" x14ac:dyDescent="0.2">
@@ -81779,10 +81779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803F4822-A3C6-9348-B33F-2B69108DF8F4}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F4" sqref="F4:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -81792,7 +81792,7 @@
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>113</v>
       </c>
@@ -81803,7 +81803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>102</v>
       </c>
@@ -81817,7 +81817,7 @@
         <v>0.35714750000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>104</v>
       </c>
@@ -81831,7 +81831,7 @@
         <v>0.36543700000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>106</v>
       </c>
@@ -81845,7 +81845,7 @@
         <v>0.216918</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>108</v>
       </c>
@@ -81859,7 +81859,7 @@
         <v>1.7813680000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>110</v>
       </c>
@@ -81872,8 +81872,10 @@
       <c r="D6">
         <v>1.3596E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>103</v>
       </c>
@@ -81884,11 +81886,12 @@
         <v>116</v>
       </c>
       <c r="D7">
-        <v>0.55777060000000001</v>
-      </c>
+        <v>0.64475850000000001</v>
+      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>105</v>
       </c>
@@ -81899,12 +81902,12 @@
         <v>116</v>
       </c>
       <c r="D8">
-        <v>0.66454760000000002</v>
+        <v>0.72718669999999996</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>107</v>
       </c>
@@ -81915,12 +81918,13 @@
         <v>116</v>
       </c>
       <c r="D9">
-        <v>0.3322329</v>
+        <v>0.3587264</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>109</v>
       </c>
@@ -81935,8 +81939,9 @@
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>111</v>
       </c>
@@ -81950,12 +81955,19 @@
         <v>-0.1076013</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" s="5"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="5"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="5"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D14" s="2"/>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.2">

</xml_diff>